<commit_message>
Recaudos Sprint CORG, AGEX y TEEX.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -359,6 +359,81 @@
   </si>
   <si>
     <t>Proceso de RECO1</t>
+  </si>
+  <si>
+    <t>vStrOpcionCarteraExt</t>
+  </si>
+  <si>
+    <t>Aged Receivables</t>
+  </si>
+  <si>
+    <t>vStrRutaCarteraDolares</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\CarteraDolares.xlsx</t>
+  </si>
+  <si>
+    <t>vStrCarteraExterior</t>
+  </si>
+  <si>
+    <t>vStrFormatoExterior</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\CarteraExterior.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\Formatos\CarteraExterior.xlsx</t>
+  </si>
+  <si>
+    <t>vStrPathAGEEX</t>
+  </si>
+  <si>
+    <t>vStRutaAGEEX</t>
+  </si>
+  <si>
+    <t>vStRutaTEEX</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\TEEX\</t>
+  </si>
+  <si>
+    <t>vstrAssetAGEEX</t>
+  </si>
+  <si>
+    <t>ArchivoAgeex</t>
+  </si>
+  <si>
+    <t>Carpeta AGEEX</t>
+  </si>
+  <si>
+    <t>vStrPathTEEX</t>
+  </si>
+  <si>
+    <t>Carpeta TEEX</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\AGEX\</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\AGEX\</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\AppData\Local\Temp</t>
+  </si>
+  <si>
+    <t>vStrRutaArchivosTemporales</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\TEX\</t>
+  </si>
+  <si>
+    <t>RutaOcnas</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\OCNA\</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\OCNA</t>
   </si>
 </sst>
 </file>
@@ -768,19 +843,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -874,250 +949,312 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
+        <v>129</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="A8" t="s">
-        <v>81</v>
+      <c r="A8" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" t="s">
-        <v>85</v>
+        <v>133</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
+      <c r="A20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>80</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2063,12 +2200,15 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$2:$C$2</xm:f>
@@ -2079,37 +2219,55 @@
           <x14:formula1>
             <xm:f>Desplegable!$B$3:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$4:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$5:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$8:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
+          <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$6:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$7:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$9:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$10:$C$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$11:$C$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2119,20 +2277,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="8" t="s">
         <v>106</v>
       </c>
@@ -2218,6 +2376,39 @@
       </c>
       <c r="C8" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2239,12 +2430,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3364,12 +3555,12 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3415,6 +3606,12 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -4439,6 +4636,7 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4450,14 +4648,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Prepagadas: Lectura de pagos de Entidadesd y realización de plantilla a cargar
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -18,12 +18,12 @@
     <sheet name="Assets" sheetId="3" r:id="rId4"/>
     <sheet name="Credentials" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="165">
   <si>
     <t>Name</t>
   </si>
@@ -434,6 +434,90 @@
   </si>
   <si>
     <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\OCNA</t>
+  </si>
+  <si>
+    <t>RutaPlantillasPREP</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\PREP\Plantillas a cargar\Plantillas generadas\</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\PREP\Plantillas a cargar\Plantillas generadas\</t>
+  </si>
+  <si>
+    <t>Ruta de folder de plantillas a cargar en prepagadas</t>
+  </si>
+  <si>
+    <t>PlantillaPREP</t>
+  </si>
+  <si>
+    <t>PLANTILLA UNICA INTERFASE.xlsx</t>
+  </si>
+  <si>
+    <t>Nombre archivo plantilla a cargar en EPICOR Prepagadas</t>
+  </si>
+  <si>
+    <t>RutaFormatoPlantillaPREP</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\Formatos\PLANTILLA UNICA INTERFASE.xlsx</t>
+  </si>
+  <si>
+    <t>Formato de Plantillas PREP</t>
+  </si>
+  <si>
+    <t>RutaReportesNuevos</t>
+  </si>
+  <si>
+    <t>C:\Users\robtireleo\Documents\Recaudos\PREP\Plantillas a cargar\Reportes nuevos\</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\PREP\Plantillas a cargar\Reportes nuevos\</t>
+  </si>
+  <si>
+    <t>Sura1</t>
+  </si>
+  <si>
+    <t>Sura Clasica</t>
+  </si>
+  <si>
+    <t>Prepagada Sura Clásica</t>
+  </si>
+  <si>
+    <t>Sura2</t>
+  </si>
+  <si>
+    <t>Sura Global</t>
+  </si>
+  <si>
+    <t>Sura3</t>
+  </si>
+  <si>
+    <t>Sura EPS PAC</t>
+  </si>
+  <si>
+    <t>Colpatria1</t>
+  </si>
+  <si>
+    <t>Axa Colpatria Original</t>
+  </si>
+  <si>
+    <t>TipoLog</t>
+  </si>
+  <si>
+    <t>Trace,Informativo,Warning,Error,Fatal</t>
+  </si>
+  <si>
+    <t>Colpatria2</t>
+  </si>
+  <si>
+    <t>Axa Colpatria Alterno</t>
+  </si>
+  <si>
+    <t>Coomeva</t>
+  </si>
+  <si>
+    <t>CasoEspCoomeva</t>
   </si>
 </sst>
 </file>
@@ -843,16 +927,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="2" max="2" width="84.21875" customWidth="1"/>
     <col min="3" max="3" width="68.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="26" width="8.6640625" customWidth="1"/>
@@ -925,352 +1009,448 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="15" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1">
+      <c r="A8" t="s">
         <v>120</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="9" spans="1:26" ht="15" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
+        <v>134</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>145</v>
+      </c>
+      <c r="C29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" t="s">
-        <v>113</v>
-      </c>
-    </row>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+        <v>164</v>
+      </c>
+      <c r="B35">
+        <v>8305337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2200,74 +2380,83 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$2:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$3:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$4:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$5:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B11</xm:sqref>
+          <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$8:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B15</xm:sqref>
+          <xm:sqref>B16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$6:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$7:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$9:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$10:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$11:$C$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B35</xm:sqref>
+          <xm:sqref>B24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$12:$C$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>B28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$13:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2277,17 +2466,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
@@ -2409,6 +2598,28 @@
       </c>
       <c r="C11" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3555,7 +3766,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Set Assets Prepagadas y Correo notificación al usuario sobre plantilla de pagos.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -18,12 +18,12 @@
     <sheet name="Assets" sheetId="3" r:id="rId4"/>
     <sheet name="Credentials" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -518,6 +518,18 @@
   </si>
   <si>
     <t>CasoEspCoomeva</t>
+  </si>
+  <si>
+    <t>Prepagadas</t>
+  </si>
+  <si>
+    <t>GrupoPREP</t>
+  </si>
+  <si>
+    <t>sergio.sanchez@fouriering.com</t>
+  </si>
+  <si>
+    <t>MailPREP</t>
   </si>
 </sst>
 </file>
@@ -929,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1317,7 +1329,14 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
         <v>150</v>
@@ -1378,7 +1397,7 @@
         <v>70</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
@@ -3766,7 +3785,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3848,7 +3867,14 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>